<commit_message>
cost per day estimate
</commit_message>
<xml_diff>
--- a/Triathlon analysis/Expense.xlsx
+++ b/Triathlon analysis/Expense.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A5BAC9-B0A8-40A0-BA4F-E80793FB5111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -70,12 +82,15 @@
   </si>
   <si>
     <t>$/day</t>
+  </si>
+  <si>
+    <t>Cost per day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -121,6 +136,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -169,7 +187,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -202,9 +220,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,6 +272,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -412,29 +464,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="A11:D11"/>
+      <selection activeCell="F11" sqref="A11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="50.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F1" s="2">
         <f>SUM(F3:F47)</f>
         <v>269.46000000000004</v>
       </c>
       <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2">
+        <f ca="1">F1/(TODAY()-A3)</f>
+        <v>8.69225806451613</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -460,7 +519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44430</v>
       </c>
@@ -485,7 +544,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44432</v>
       </c>
@@ -510,7 +569,7 @@
         <v>28.08</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44440</v>
       </c>
@@ -535,7 +594,7 @@
         <v>7.7140000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44445</v>
       </c>
@@ -560,7 +619,7 @@
         <v>5.8486666666666673</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44447</v>
       </c>
@@ -585,7 +644,7 @@
         <v>9.5758823529411785</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44449</v>
       </c>
@@ -610,7 +669,7 @@
         <v>11.404736842105265</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44454</v>
       </c>
@@ -635,7 +694,7 @@
         <v>10.750833333333334</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44453</v>
       </c>
@@ -660,19 +719,16 @@
         <v>11.715652173913044</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="D11" s="2"/>
-      <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2">
         <f>SUM($D$3:D11)/(A11-$A$3)</f>
         <v>-6.0648210668467258E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
@@ -683,7 +739,7 @@
         <v>-6.0648210668467258E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
@@ -694,7 +750,7 @@
         <v>-6.0648210668467258E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
@@ -705,7 +761,7 @@
         <v>-6.0648210668467258E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
@@ -716,7 +772,7 @@
         <v>-6.0648210668467258E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
@@ -1070,12 +1126,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1087,7 +1143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Added TacX flow refund
</commit_message>
<xml_diff>
--- a/Triathlon analysis/Expense.xlsx
+++ b/Triathlon analysis/Expense.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Equipment</t>
+  </si>
+  <si>
+    <t>TacX Flow refund</t>
+  </si>
+  <si>
+    <t>UPS refunded the seller because the package was damaged and missing components, she then gave me the price less shipping back.</t>
   </si>
 </sst>
 </file>
@@ -438,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,13 +453,15 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="50.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F1" s="2">
         <f>SUM(F3:F47)</f>
-        <v>502.66</v>
+        <v>302.66000000000003</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" t="s">
@@ -461,7 +469,7 @@
       </c>
       <c r="I1" s="2">
         <f ca="1">F1/(TODAY()-A3)</f>
-        <v>15.708125000000001</v>
+        <v>5.8203846153846159</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -533,7 +541,7 @@
         <v>14.83</v>
       </c>
       <c r="G4" s="2">
-        <f>SUM($D$3:D4)/(A4-$A$3)</f>
+        <f>SUM($F$3:F4)/(A4-$A$3)</f>
         <v>28.08</v>
       </c>
       <c r="H4" t="s">
@@ -561,7 +569,7 @@
         <v>20.98</v>
       </c>
       <c r="G5" s="2">
-        <f>SUM($D$3:D5)/(A5-$A$3)</f>
+        <f>SUM($F$3:F5)/(A5-$A$3)</f>
         <v>7.7140000000000004</v>
       </c>
     </row>
@@ -586,7 +594,7 @@
         <v>10.59</v>
       </c>
       <c r="G6" s="2">
-        <f>SUM($D$3:D6)/(A6-$A$3)</f>
+        <f>SUM($F$3:F6)/(A6-$A$3)</f>
         <v>5.8486666666666673</v>
       </c>
     </row>
@@ -611,7 +619,7 @@
         <v>75.06</v>
       </c>
       <c r="G7" s="2">
-        <f>SUM($D$3:D7)/(A7-$A$3)</f>
+        <f>SUM($F$3:F7)/(A7-$A$3)</f>
         <v>9.5758823529411785</v>
       </c>
     </row>
@@ -636,7 +644,7 @@
         <v>53.9</v>
       </c>
       <c r="G8" s="2">
-        <f>SUM($D$3:D8)/(A8-$A$3)</f>
+        <f>SUM($F$3:F8)/(A8-$A$3)</f>
         <v>11.404736842105265</v>
       </c>
     </row>
@@ -661,7 +669,7 @@
         <v>41.33</v>
       </c>
       <c r="G9" s="2">
-        <f>SUM($D$3:D9)/(A9-$A$3)</f>
+        <f>SUM($F$3:F9)/(A9-$A$3)</f>
         <v>10.750833333333334</v>
       </c>
     </row>
@@ -686,7 +694,7 @@
         <v>11.44</v>
       </c>
       <c r="G10" s="2">
-        <f>SUM($D$3:D10)/(A10-$A$3)</f>
+        <f>SUM($F$3:F10)/(A10-$A$3)</f>
         <v>11.715652173913044</v>
       </c>
     </row>
@@ -711,19 +719,36 @@
         <v>233.2</v>
       </c>
       <c r="G11" s="2">
-        <f>SUM($D$3:D11)/(A11-$A$3)</f>
+        <f>SUM($F$3:F11)/(A11-$A$3)</f>
         <v>15.708125000000001</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="2"/>
+      <c r="A12" s="1">
+        <v>44481</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-200</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-200</v>
       </c>
       <c r="G12" s="2">
-        <f>SUM($D$3:D12)/(A12-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F12)/(A12-$A$3)</f>
+        <v>5.9345098039215687</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -733,8 +758,8 @@
         <v>0</v>
       </c>
       <c r="G13" s="2">
-        <f>SUM($D$3:D13)/(A13-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F13)/(A13-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -744,8 +769,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="2">
-        <f>SUM($D$3:D14)/(A14-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F14)/(A14-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -755,8 +780,8 @@
         <v>0</v>
       </c>
       <c r="G15" s="2">
-        <f>SUM($D$3:D15)/(A15-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F15)/(A15-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -766,8 +791,8 @@
         <v>0</v>
       </c>
       <c r="G16" s="2">
-        <f>SUM($D$3:D16)/(A16-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F16)/(A16-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
@@ -777,8 +802,8 @@
         <v>0</v>
       </c>
       <c r="G17" s="2">
-        <f>SUM($D$3:D17)/(A17-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F17)/(A17-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
@@ -788,8 +813,8 @@
         <v>0</v>
       </c>
       <c r="G18" s="2">
-        <f>SUM($D$3:D18)/(A18-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F18)/(A18-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
@@ -799,8 +824,8 @@
         <v>0</v>
       </c>
       <c r="G19" s="2">
-        <f>SUM($D$3:D19)/(A19-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F19)/(A19-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
@@ -810,8 +835,8 @@
         <v>0</v>
       </c>
       <c r="G20" s="2">
-        <f>SUM($D$3:D20)/(A20-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F20)/(A20-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
@@ -821,8 +846,8 @@
         <v>0</v>
       </c>
       <c r="G21" s="2">
-        <f>SUM($D$3:D21)/(A21-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F21)/(A21-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
@@ -832,8 +857,8 @@
         <v>0</v>
       </c>
       <c r="G22" s="2">
-        <f>SUM($D$3:D22)/(A22-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F22)/(A22-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
@@ -843,8 +868,8 @@
         <v>0</v>
       </c>
       <c r="G23" s="2">
-        <f>SUM($D$3:D23)/(A23-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F23)/(A23-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
@@ -854,8 +879,8 @@
         <v>0</v>
       </c>
       <c r="G24" s="2">
-        <f>SUM($D$3:D24)/(A24-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F24)/(A24-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
@@ -865,8 +890,8 @@
         <v>0</v>
       </c>
       <c r="G25" s="2">
-        <f>SUM($D$3:D25)/(A25-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F25)/(A25-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
@@ -876,8 +901,8 @@
         <v>0</v>
       </c>
       <c r="G26" s="2">
-        <f>SUM($D$3:D26)/(A26-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F26)/(A26-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.25">
@@ -887,8 +912,8 @@
         <v>0</v>
       </c>
       <c r="G27" s="2">
-        <f>SUM($D$3:D27)/(A27-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F27)/(A27-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.25">
@@ -898,8 +923,8 @@
         <v>0</v>
       </c>
       <c r="G28" s="2">
-        <f>SUM($D$3:D28)/(A28-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F28)/(A28-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.25">
@@ -909,8 +934,8 @@
         <v>0</v>
       </c>
       <c r="G29" s="2">
-        <f>SUM($D$3:D29)/(A29-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F29)/(A29-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
@@ -920,8 +945,8 @@
         <v>0</v>
       </c>
       <c r="G30" s="2">
-        <f>SUM($D$3:D30)/(A30-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F30)/(A30-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
@@ -931,8 +956,8 @@
         <v>0</v>
       </c>
       <c r="G31" s="2">
-        <f>SUM($D$3:D31)/(A31-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F31)/(A31-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
@@ -942,8 +967,8 @@
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <f>SUM($D$3:D32)/(A32-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F32)/(A32-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.25">
@@ -953,8 +978,8 @@
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <f>SUM($D$3:D33)/(A33-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F33)/(A33-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.25">
@@ -964,8 +989,8 @@
         <v>0</v>
       </c>
       <c r="G34" s="2">
-        <f>SUM($D$3:D34)/(A34-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F34)/(A34-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.25">
@@ -975,8 +1000,8 @@
         <v>0</v>
       </c>
       <c r="G35" s="2">
-        <f>SUM($D$3:D35)/(A35-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F35)/(A35-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.25">
@@ -986,8 +1011,8 @@
         <v>0</v>
       </c>
       <c r="G36" s="2">
-        <f>SUM($D$3:D36)/(A36-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F36)/(A36-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.25">
@@ -997,8 +1022,8 @@
         <v>0</v>
       </c>
       <c r="G37" s="2">
-        <f>SUM($D$3:D37)/(A37-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F37)/(A37-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
@@ -1008,8 +1033,8 @@
         <v>0</v>
       </c>
       <c r="G38" s="2">
-        <f>SUM($D$3:D38)/(A38-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F38)/(A38-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.25">
@@ -1019,8 +1044,8 @@
         <v>0</v>
       </c>
       <c r="G39" s="2">
-        <f>SUM($D$3:D39)/(A39-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F39)/(A39-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.25">
@@ -1030,8 +1055,8 @@
         <v>0</v>
       </c>
       <c r="G40" s="2">
-        <f>SUM($D$3:D40)/(A40-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F40)/(A40-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.25">
@@ -1041,8 +1066,8 @@
         <v>0</v>
       </c>
       <c r="G41" s="2">
-        <f>SUM($D$3:D41)/(A41-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F41)/(A41-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="42" spans="4:7" x14ac:dyDescent="0.25">
@@ -1052,8 +1077,8 @@
         <v>0</v>
       </c>
       <c r="G42" s="2">
-        <f>SUM($D$3:D42)/(A42-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F42)/(A42-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="43" spans="4:7" x14ac:dyDescent="0.25">
@@ -1063,8 +1088,8 @@
         <v>0</v>
       </c>
       <c r="G43" s="2">
-        <f>SUM($D$3:D43)/(A43-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F43)/(A43-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.25">
@@ -1074,8 +1099,8 @@
         <v>0</v>
       </c>
       <c r="G44" s="2">
-        <f>SUM($D$3:D44)/(A44-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F44)/(A44-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.25">
@@ -1085,8 +1110,8 @@
         <v>0</v>
       </c>
       <c r="G45" s="2">
-        <f>SUM($D$3:D45)/(A45-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F45)/(A45-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="46" spans="4:7" x14ac:dyDescent="0.25">
@@ -1096,8 +1121,8 @@
         <v>0</v>
       </c>
       <c r="G46" s="2">
-        <f>SUM($D$3:D46)/(A46-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F46)/(A46-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
     <row r="47" spans="4:7" x14ac:dyDescent="0.25">
@@ -1107,8 +1132,8 @@
         <v>0</v>
       </c>
       <c r="G47" s="2">
-        <f>SUM($D$3:D47)/(A47-$A$3)</f>
-        <v>-1.1313526896241278E-2</v>
+        <f>SUM($F$3:F47)/(A47-$A$3)</f>
+        <v>-6.8120639207742521E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>